<commit_message>
Some touches on the model
- adicionei um motor
-adicionei um drivecycle mais longo
</commit_message>
<xml_diff>
--- a/Documents/Motors_List.xlsx
+++ b/Documents/Motors_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmeni\Documents\GitHub\Powertrain-ISTrain-24_25\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567A643A-D133-4E73-86FE-39DB6283EFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC953DE4-F2AE-45BD-B380-9E72AC93B005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77B3B303-ED70-45CA-AA46-843829307B1E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{77B3B303-ED70-45CA-AA46-843829307B1E}"/>
   </bookViews>
   <sheets>
     <sheet name="DC motor" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="60">
   <si>
     <t>-</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Weigth</t>
   </si>
   <si>
-    <t>https://tinyurl.com/2xbnh8y8</t>
-  </si>
-  <si>
     <t>150(5)</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
   </si>
   <si>
     <t>https://tinyurl.com/2ptbsjsy</t>
-  </si>
-  <si>
-    <t>https://tinyurl.com/47xpvxkr</t>
   </si>
   <si>
     <t>yes</t>
@@ -192,6 +186,43 @@
   <si>
     <t>1-Tem colling
 2-Tem controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tinyurl.com/47xpvxkr </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tinyurl.com/2xbnh8y8 </t>
+  </si>
+  <si>
+    <t>Peak Power(kW)</t>
+  </si>
+  <si>
+    <t>Nominal Power(kW)</t>
+  </si>
+  <si>
+    <t>Peak Torque(N.m)</t>
+  </si>
+  <si>
+    <t>Nominal Torque(N.m)</t>
+  </si>
+  <si>
+    <t>Nominal Current(A)</t>
+  </si>
+  <si>
+    <t>Nominal Voltage(V)</t>
+  </si>
+  <si>
+    <t>Peak Speed (rpm)</t>
+  </si>
+  <si>
+    <t>Nominal speed(rpm)</t>
+  </si>
+  <si>
+    <t>Price(€)</t>
+  </si>
+  <si>
+    <t>1.Tem sensor de temperatura imbutido
+2.Tem bastante technical info available</t>
   </si>
 </sst>
 </file>
@@ -602,7 +633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D596B62-309F-449B-AFFC-ECE36077CC4B}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -686,7 +717,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -825,22 +856,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6B312E-22D5-4601-A971-E432CD754561}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="41.33203125" customWidth="1"/>
@@ -857,37 +889,37 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>31</v>
@@ -906,14 +938,14 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>32</v>
+      <c r="C2" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E2">
         <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -946,24 +978,24 @@
         <v>5</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>500</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -978,7 +1010,7 @@
         <v>9.4</v>
       </c>
       <c r="K3">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L3">
         <v>48</v>
@@ -994,6 +1026,9 @@
       </c>
       <c r="P3" t="s">
         <v>4</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -1003,14 +1038,14 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>37</v>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="E4">
         <v>350</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1019,13 +1054,13 @@
         <v>1.5</v>
       </c>
       <c r="I4">
-        <v>8</v>
-      </c>
-      <c r="J4">
         <v>5</v>
       </c>
-      <c r="K4" t="s">
-        <v>0</v>
+      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>20</v>
       </c>
       <c r="L4">
         <v>48</v>
@@ -1034,30 +1069,30 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>4100</v>
+        <v>3000</v>
       </c>
       <c r="O4">
         <v>4.9000000000000004</v>
       </c>
       <c r="P4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>200</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5">
         <v>5.2</v>
@@ -1092,22 +1127,22 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6">
         <v>270</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6">
         <v>5.2</v>
@@ -1145,6 +1180,8 @@
     <hyperlink ref="C6" r:id="rId1" xr:uid="{52D3AC2E-737B-4DAE-9975-85F9308F4234}"/>
     <hyperlink ref="C5" r:id="rId2" xr:uid="{093E079C-7759-4C29-89AA-DA4E6640C552}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{D8260F19-E8A1-4A19-B8A2-28B4194D47A3}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{484F376E-163C-4B8B-9E50-2E6E7DCFA387}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{D47C5DBD-0CB0-4EFE-AB89-85EDE46F3D01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1186,7 +1223,7 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -1230,13 +1267,13 @@
     </row>
     <row r="2" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1263,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M2">
         <v>3000</v>
@@ -1275,7 +1312,7 @@
         <v>27</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>